<commit_message>
HOT-27 - Saving optimizer comparison.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database comparison.xlsx
+++ b/hotrod/docs/research/database comparison.xlsx
@@ -103,13 +103,13 @@
     <t xml:space="preserve">Case Less *3</t>
   </si>
   <si>
-    <t xml:space="preserve">None *4</t>
+    <t xml:space="preserve">Sensitive *4</t>
   </si>
   <si>
     <t xml:space="preserve">Key Generation</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequences</t>
+    <t xml:space="preserve">Sequences available</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -172,7 +172,7 @@
     <t xml:space="preserve">Yes *10</t>
   </si>
   <si>
-    <t xml:space="preserve">Yes *12</t>
+    <t xml:space="preserve">Since 5.7</t>
   </si>
   <si>
     <t xml:space="preserve">Indexes on Virtual Columns</t>
@@ -232,7 +232,7 @@
     <t xml:space="preserve">*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
   </si>
   <si>
-    <t xml:space="preserve">*2 Not used internally.</t>
+    <t xml:space="preserve">*2 Informed by the database, but not used internally.</t>
   </si>
   <si>
     <t xml:space="preserve">*3 The identifier can be typed in any case. It will match other cases.</t>
@@ -262,7 +262,7 @@
     <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
   </si>
   <si>
-    <t xml:space="preserve">*12 Since MySQL 5.7</t>
+    <t xml:space="preserve">*12 </t>
   </si>
   <si>
     <t xml:space="preserve">*13 Always persisted.</t>
@@ -555,7 +555,7 @@
   <dimension ref="A1:K43"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>

<commit_message>
HOT-27 - H2 hierarchical queries.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database comparison.xlsx
+++ b/hotrod/docs/research/database comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="86">
   <si>
     <t xml:space="preserve">High End</t>
   </si>
@@ -151,6 +151,9 @@
     <t xml:space="preserve">From 8.0</t>
   </si>
   <si>
+    <t xml:space="preserve">Yes *12</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Expressions</t>
   </si>
   <si>
@@ -262,7 +265,7 @@
     <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
   </si>
   <si>
-    <t xml:space="preserve">*12 </t>
+    <t xml:space="preserve">*12 Cannot create views with hierarchical queries.</t>
   </si>
   <si>
     <t xml:space="preserve">*13 Always persisted.</t>
@@ -560,15 +563,15 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="32.3979591836735"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.7448979591837"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4744897959184"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -966,11 +969,13 @@
         <v>31</v>
       </c>
       <c r="J12" s="8"/>
-      <c r="K12" s="8"/>
+      <c r="K12" s="10" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>30</v>
@@ -997,10 +1002,10 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>31</v>
@@ -1024,26 +1029,26 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="7" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="E15" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="8"/>
       <c r="G15" s="10" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="H15" s="10" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="I15" s="9"/>
       <c r="J15" s="8"/>
@@ -1051,7 +1056,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -1067,7 +1072,7 @@
       </c>
       <c r="F16" s="8"/>
       <c r="G16" s="10" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="H16" s="10" t="s">
         <v>30</v>
@@ -1078,7 +1083,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1093,7 +1098,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
         <v>4</v>
@@ -1128,7 +1133,7 @@
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>30</v>
@@ -1143,7 +1148,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G19" s="10" t="s">
         <v>30</v>
@@ -1163,22 +1168,22 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D20" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E20" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F20" s="8" t="s">
         <v>57</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F20" s="8" t="s">
-        <v>56</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>30</v>
@@ -1198,7 +1203,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B21" s="10" t="s">
         <v>30</v>
@@ -1207,19 +1212,19 @@
         <v>30</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="E21" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G21" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H21" s="14" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="I21" s="13" t="s">
         <v>31</v>
@@ -1233,7 +1238,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B22" s="10" t="s">
         <v>30</v>
@@ -1248,7 +1253,7 @@
         <v>30</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>31</v>
@@ -1268,7 +1273,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>30</v>
@@ -1283,13 +1288,13 @@
         <v>31</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G23" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="H23" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I23" s="9"/>
       <c r="J23" s="8"/>
@@ -1297,28 +1302,28 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F24" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G24" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="H24" s="14" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="8"/>
@@ -1326,13 +1331,13 @@
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B25" s="12" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="14" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D25" s="13" t="s">
         <v>31</v>
@@ -1341,7 +1346,7 @@
         <v>30</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G25" s="12" t="s">
         <v>31</v>
@@ -1355,7 +1360,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B26" s="10" t="s">
         <v>30</v>
@@ -1370,7 +1375,7 @@
         <v>30</v>
       </c>
       <c r="F26" s="8" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="G26" s="12" t="s">
         <v>31</v>
@@ -1387,84 +1392,84 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="K29" s="16"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT-27 - DB comparison updated.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database comparison.xlsx
+++ b/hotrod/docs/research/database comparison.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="91">
   <si>
     <t xml:space="preserve">High End</t>
   </si>
@@ -100,7 +100,7 @@
     <t xml:space="preserve">lower</t>
   </si>
   <si>
-    <t xml:space="preserve">Case Less *3</t>
+    <t xml:space="preserve">Insensitive *3</t>
   </si>
   <si>
     <t xml:space="preserve">Sensitive *4</t>
@@ -109,7 +109,7 @@
     <t xml:space="preserve">Key Generation</t>
   </si>
   <si>
-    <t xml:space="preserve">Sequences available</t>
+    <t xml:space="preserve">Sequences</t>
   </si>
   <si>
     <t xml:space="preserve">Yes</t>
@@ -145,6 +145,9 @@
     <t xml:space="preserve">Yes *7</t>
   </si>
   <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
     <t xml:space="preserve">Since 10.2.2</t>
   </si>
   <si>
@@ -154,6 +157,30 @@
     <t xml:space="preserve">Yes *12</t>
   </si>
   <si>
+    <t xml:space="preserve">Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Text Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Optimization</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indexes on Expressions</t>
   </si>
   <si>
@@ -163,28 +190,34 @@
     <t xml:space="preserve">Yes *16</t>
   </si>
   <si>
-    <t xml:space="preserve">Virtual Columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since 5.7</t>
-  </si>
-  <si>
     <t xml:space="preserve">Indexes on Virtual Columns</t>
   </si>
   <si>
     <t xml:space="preserve">Yes *11</t>
   </si>
   <si>
-    <t xml:space="preserve">Full Text Search</t>
+    <t xml:space="preserve">Optional indexes on FKs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Organized Tables (no heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Indexes (data in heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-key columns on Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Indexes</t>
   </si>
   <si>
     <t xml:space="preserve">SQL Optimization</t>
@@ -193,9 +226,6 @@
     <t xml:space="preserve">Explain Plan</t>
   </si>
   <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
     <t xml:space="preserve">Explain Plan without execution</t>
   </si>
   <si>
@@ -211,27 +241,6 @@
     <t xml:space="preserve">Yes *6</t>
   </si>
   <si>
-    <t xml:space="preserve">Optional indexes on FKs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index Organized Tables (IOTs)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clustered Indexes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-key columns on Indexes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial Indexes</t>
-  </si>
-  <si>
     <t xml:space="preserve">*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
   </si>
   <si>
@@ -265,7 +274,7 @@
     <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
   </si>
   <si>
-    <t xml:space="preserve">*12 Cannot create views with hierarchical queries.</t>
+    <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
   </si>
   <si>
     <t xml:space="preserve">*13 Always persisted.</t>
@@ -278,6 +287,12 @@
   </si>
   <si>
     <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*18 Are always persistent columns.</t>
   </si>
 </sst>
 </file>
@@ -555,23 +570,24 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:K43"/>
+  <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.9948979591837"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.4744897959184"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5867346938776"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.25"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1326530612245"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -958,105 +974,113 @@
       <c r="E12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8"/>
+      <c r="F12" s="8" t="s">
+        <v>41</v>
+      </c>
       <c r="G12" s="10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H12" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I12" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="J12" s="10" t="s">
+        <v>30</v>
+      </c>
       <c r="K12" s="10" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>30</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="F13" s="8"/>
-      <c r="G13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I13" s="9"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+        <v>46</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>47</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="H13" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="C14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>31</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="8"/>
       <c r="F14" s="8"/>
-      <c r="G14" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H14" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
       <c r="I14" s="9"/>
       <c r="J14" s="8"/>
       <c r="K14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="D15" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="E15" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="8"/>
-      <c r="G15" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H15" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="I15" s="9"/>
-      <c r="J15" s="8"/>
-      <c r="K15" s="8"/>
+      <c r="A15" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -1064,76 +1088,104 @@
       <c r="C16" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="H16" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" s="9"/>
-      <c r="J16" s="8"/>
-      <c r="K16" s="8"/>
+      <c r="D16" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I16" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J16" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="8"/>
-      <c r="I17" s="9"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="B17" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J17" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K17" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="4" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="E18" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="G18" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I18" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="J18" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K18" s="5" t="s">
-        <v>13</v>
+      <c r="A18" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K18" s="10" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="7" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
         <v>30</v>
@@ -1148,112 +1200,112 @@
         <v>30</v>
       </c>
       <c r="F19" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="G19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I19" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J19" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K19" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="7" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D20" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E20" s="10" t="s">
-        <v>30</v>
+      <c r="C20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E20" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="F20" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" s="10" t="s">
-        <v>30</v>
+        <v>41</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>60</v>
       </c>
       <c r="I20" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="J20" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" s="10" t="s">
-        <v>30</v>
+      <c r="J20" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K20" s="12" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>30</v>
+        <v>61</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="C21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E21" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G21" s="14" t="s">
         <v>60</v>
       </c>
-      <c r="E21" s="14" t="s">
-        <v>61</v>
-      </c>
-      <c r="F21" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G21" s="14" t="s">
+      <c r="H21" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="I21" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J21" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K21" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="H21" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="I21" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J21" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" s="10" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="B22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D22" s="11" t="s">
-        <v>30</v>
+      <c r="B22" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="13" t="s">
+        <v>31</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>31</v>
@@ -1273,203 +1325,272 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C23" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="12" t="s">
-        <v>31</v>
+      <c r="C23" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D23" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H23" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="8"/>
-      <c r="K23" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="G23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="I23" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J23" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K23" s="12" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="7" t="s">
+      <c r="A24" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B24" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E24" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F24" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="B24" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F24" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K24" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="7" t="s">
         <v>67</v>
       </c>
-      <c r="B25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="D25" s="13" t="s">
-        <v>31</v>
+      <c r="B25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D25" s="11" t="s">
+        <v>30</v>
       </c>
       <c r="E25" s="10" t="s">
         <v>30</v>
       </c>
       <c r="F25" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H25" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="8"/>
-      <c r="K25" s="8"/>
+        <v>41</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I25" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K25" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="H26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F26" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="G26" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="H26" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="8"/>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="K27" s="0"/>
-    </row>
-    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="0" t="s">
+      <c r="B27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="K28" s="0"/>
+      <c r="E27" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F27" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="G27" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H27" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I27" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="K29" s="16"/>
+      <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>72</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="K30" s="0"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>73</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="K31" s="16"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="s">
+        <v>90</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
HOT-27 - Adding SAP ASE details.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database comparison.xlsx
+++ b/hotrod/docs/research/database comparison.xlsx
@@ -22,277 +22,277 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="91">
   <si>
-    <t xml:space="preserve">High End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Middle Tier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lighweight Tier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Organization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oracle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DB2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PostgreSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL Server</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SAP ASE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MariaDB</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MySQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Derby</t>
-  </si>
-  <si>
-    <t xml:space="preserve">HyperSQL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Catalog Term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">database *2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">database</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CATALOG *2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">catalog *2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Schema Term</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schema</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SCHEMA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identifier default case</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UPPER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lower</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Insensitive *3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sensitive *4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Key Generation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sequences</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identities generated always</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since 12c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identities generated by default</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identity columns per table</t>
-  </si>
-  <si>
-    <t xml:space="preserve">single</t>
-  </si>
-  <si>
-    <t xml:space="preserve">multiple</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Features</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hierarchical Queries</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since 10.2.2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">From 8.0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *12</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Virtual Columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *15</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *10</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Since 5.7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *18</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Full Text Search</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index Optimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indexes on Expressions</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indexes on Expressions with UDF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *16</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indexes on Virtual Columns</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *11</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Optional indexes on FKs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Index Organized Tables (no heap)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clustered Indexes (data in heap)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *17</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Non-key columns on Indexes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Partial Indexes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SQL Optimization</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explain Plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explain Plan without execution</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Explain Plan with parameters</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes *6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*2 Informed by the database, but not used internally.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*3 The identifier can be typed in any case. It will match other cases.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*4 The identifier will be stored in the case it was typed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*5 Yes, but the parameter types must be specified (not the values).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*7 Not enabled by default. The DBA needs to enable them after installation.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*8 On unique indexes only.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*9 Only on InnoDB tables.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*10 Can use user-defined functions since 10.2.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*13 Always persisted.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*14 User-defined functions are not allowed.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*18 Are always persistent columns.</t>
+    <t>High End</t>
+  </si>
+  <si>
+    <t>Middle Tier</t>
+  </si>
+  <si>
+    <t>Lighweight Tier</t>
+  </si>
+  <si>
+    <t>Organization</t>
+  </si>
+  <si>
+    <t>Oracle</t>
+  </si>
+  <si>
+    <t>DB2</t>
+  </si>
+  <si>
+    <t>PostgreSQL</t>
+  </si>
+  <si>
+    <t>SQL Server</t>
+  </si>
+  <si>
+    <t>SAP ASE</t>
+  </si>
+  <si>
+    <t>MariaDB</t>
+  </si>
+  <si>
+    <t>MySQL</t>
+  </si>
+  <si>
+    <t>Derby</t>
+  </si>
+  <si>
+    <t>HyperSQL</t>
+  </si>
+  <si>
+    <t>H2</t>
+  </si>
+  <si>
+    <t>Catalog Term</t>
+  </si>
+  <si>
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>database *2</t>
+  </si>
+  <si>
+    <t>database</t>
+  </si>
+  <si>
+    <t>CATALOG *2</t>
+  </si>
+  <si>
+    <t>catalog *2</t>
+  </si>
+  <si>
+    <t>Schema Term</t>
+  </si>
+  <si>
+    <t>schema</t>
+  </si>
+  <si>
+    <t>SCHEMA</t>
+  </si>
+  <si>
+    <t>Identifier default case</t>
+  </si>
+  <si>
+    <t>UPPER</t>
+  </si>
+  <si>
+    <t>lower</t>
+  </si>
+  <si>
+    <t>Insensitive *3</t>
+  </si>
+  <si>
+    <t>Sensitive *4</t>
+  </si>
+  <si>
+    <t>Key Generation</t>
+  </si>
+  <si>
+    <t>Sequences</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Identities generated always</t>
+  </si>
+  <si>
+    <t>Since 12c</t>
+  </si>
+  <si>
+    <t>Identities generated by default</t>
+  </si>
+  <si>
+    <t>Identity columns per table</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>multiple</t>
+  </si>
+  <si>
+    <t>Features</t>
+  </si>
+  <si>
+    <t>Hierarchical Queries</t>
+  </si>
+  <si>
+    <t>Yes *7</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>Since 10.2.2</t>
+  </si>
+  <si>
+    <t>From 8.0</t>
+  </si>
+  <si>
+    <t>Yes *12</t>
+  </si>
+  <si>
+    <t>Virtual Columns</t>
+  </si>
+  <si>
+    <t>Yes *13</t>
+  </si>
+  <si>
+    <t>Yes *15</t>
+  </si>
+  <si>
+    <t>Yes *10</t>
+  </si>
+  <si>
+    <t>Since 5.7</t>
+  </si>
+  <si>
+    <t>Yes *18</t>
+  </si>
+  <si>
+    <t>Full Text Search</t>
+  </si>
+  <si>
+    <t>Index Optimization</t>
+  </si>
+  <si>
+    <t>Indexes on Expressions</t>
+  </si>
+  <si>
+    <t>Indexes on Expressions with UDF</t>
+  </si>
+  <si>
+    <t>Yes *16</t>
+  </si>
+  <si>
+    <t>Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t>Yes *11</t>
+  </si>
+  <si>
+    <t>Optional indexes on FKs</t>
+  </si>
+  <si>
+    <t>Index Organized Tables (no heap)</t>
+  </si>
+  <si>
+    <t>Yes *9</t>
+  </si>
+  <si>
+    <t>Clustered Indexes (data in heap)</t>
+  </si>
+  <si>
+    <t>Yes *17</t>
+  </si>
+  <si>
+    <t>Non-key columns on Indexes</t>
+  </si>
+  <si>
+    <t>Yes *8</t>
+  </si>
+  <si>
+    <t>Partial Indexes</t>
+  </si>
+  <si>
+    <t>SQL Optimization</t>
+  </si>
+  <si>
+    <t>Explain Plan</t>
+  </si>
+  <si>
+    <t>Explain Plan without execution</t>
+  </si>
+  <si>
+    <t>Explain Plan with parameters</t>
+  </si>
+  <si>
+    <t>Yes *1</t>
+  </si>
+  <si>
+    <t>Yes *5</t>
+  </si>
+  <si>
+    <t>Yes *6</t>
+  </si>
+  <si>
+    <t>*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
+  </si>
+  <si>
+    <t>*2 Informed by the database, but not used internally.</t>
+  </si>
+  <si>
+    <t>*3 The identifier can be typed in any case. It will match other cases.</t>
+  </si>
+  <si>
+    <t>*4 The identifier will be stored in the case it was typed.</t>
+  </si>
+  <si>
+    <t>*5 Yes, but the parameter types must be specified (not the values).</t>
+  </si>
+  <si>
+    <t>*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
+  </si>
+  <si>
+    <t>*7 Not enabled by default. The DBA needs to enable them after installation.</t>
+  </si>
+  <si>
+    <t>*8 On unique indexes only.</t>
+  </si>
+  <si>
+    <t>*9 Only on InnoDB tables.</t>
+  </si>
+  <si>
+    <t>*10 Can use user-defined functions since 10.2.1</t>
+  </si>
+  <si>
+    <t>*11 Only persistent virtual columns can be indexed.</t>
+  </si>
+  <si>
+    <t>*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
+  </si>
+  <si>
+    <t>*13 Always persisted.</t>
+  </si>
+  <si>
+    <t>*14 User-defined functions are not allowed.</t>
+  </si>
+  <si>
+    <t>*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
+  </si>
+  <si>
+    <t>*16 Must use deterministic UDFs.</t>
+  </si>
+  <si>
+    <t>*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
+  </si>
+  <si>
+    <t>*18 Are always persistent columns.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +300,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="164" formatCode="GENERAL"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -573,21 +573,22 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F14" activeCellId="0" sqref="F14"/>
+      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.5867346938776"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.25"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1326530612245"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.2857142857143"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1094,8 +1095,8 @@
       <c r="E16" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F16" s="8" t="s">
-        <v>41</v>
+      <c r="F16" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G16" s="12" t="s">
         <v>31</v>
@@ -1497,6 +1498,9 @@
       <c r="K27" s="10" t="s">
         <v>30</v>
       </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="K29" s="0"/>

</xml_diff>

<commit_message>
HOT-27 - Adding SAP ASE feature sheet.
</commit_message>
<xml_diff>
--- a/hotrod/docs/research/database comparison.xlsx
+++ b/hotrod/docs/research/database comparison.xlsx
@@ -20,279 +20,282 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="91">
-  <si>
-    <t>High End</t>
-  </si>
-  <si>
-    <t>Middle Tier</t>
-  </si>
-  <si>
-    <t>Lighweight Tier</t>
-  </si>
-  <si>
-    <t>Organization</t>
-  </si>
-  <si>
-    <t>Oracle</t>
-  </si>
-  <si>
-    <t>DB2</t>
-  </si>
-  <si>
-    <t>PostgreSQL</t>
-  </si>
-  <si>
-    <t>SQL Server</t>
-  </si>
-  <si>
-    <t>SAP ASE</t>
-  </si>
-  <si>
-    <t>MariaDB</t>
-  </si>
-  <si>
-    <t>MySQL</t>
-  </si>
-  <si>
-    <t>Derby</t>
-  </si>
-  <si>
-    <t>HyperSQL</t>
-  </si>
-  <si>
-    <t>H2</t>
-  </si>
-  <si>
-    <t>Catalog Term</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>database *2</t>
-  </si>
-  <si>
-    <t>database</t>
-  </si>
-  <si>
-    <t>CATALOG *2</t>
-  </si>
-  <si>
-    <t>catalog *2</t>
-  </si>
-  <si>
-    <t>Schema Term</t>
-  </si>
-  <si>
-    <t>schema</t>
-  </si>
-  <si>
-    <t>SCHEMA</t>
-  </si>
-  <si>
-    <t>Identifier default case</t>
-  </si>
-  <si>
-    <t>UPPER</t>
-  </si>
-  <si>
-    <t>lower</t>
-  </si>
-  <si>
-    <t>Insensitive *3</t>
-  </si>
-  <si>
-    <t>Sensitive *4</t>
-  </si>
-  <si>
-    <t>Key Generation</t>
-  </si>
-  <si>
-    <t>Sequences</t>
-  </si>
-  <si>
-    <t>Yes</t>
-  </si>
-  <si>
-    <t>No</t>
-  </si>
-  <si>
-    <t>Identities generated always</t>
-  </si>
-  <si>
-    <t>Since 12c</t>
-  </si>
-  <si>
-    <t>Identities generated by default</t>
-  </si>
-  <si>
-    <t>Identity columns per table</t>
-  </si>
-  <si>
-    <t>single</t>
-  </si>
-  <si>
-    <t>multiple</t>
-  </si>
-  <si>
-    <t>Features</t>
-  </si>
-  <si>
-    <t>Hierarchical Queries</t>
-  </si>
-  <si>
-    <t>Yes *7</t>
-  </si>
-  <si>
-    <t>?</t>
-  </si>
-  <si>
-    <t>Since 10.2.2</t>
-  </si>
-  <si>
-    <t>From 8.0</t>
-  </si>
-  <si>
-    <t>Yes *12</t>
-  </si>
-  <si>
-    <t>Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *13</t>
-  </si>
-  <si>
-    <t>Yes *15</t>
-  </si>
-  <si>
-    <t>Yes *10</t>
-  </si>
-  <si>
-    <t>Since 5.7</t>
-  </si>
-  <si>
-    <t>Yes *18</t>
-  </si>
-  <si>
-    <t>Full Text Search</t>
-  </si>
-  <si>
-    <t>Index Optimization</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions</t>
-  </si>
-  <si>
-    <t>Indexes on Expressions with UDF</t>
-  </si>
-  <si>
-    <t>Yes *16</t>
-  </si>
-  <si>
-    <t>Indexes on Virtual Columns</t>
-  </si>
-  <si>
-    <t>Yes *11</t>
-  </si>
-  <si>
-    <t>Optional indexes on FKs</t>
-  </si>
-  <si>
-    <t>Index Organized Tables (no heap)</t>
-  </si>
-  <si>
-    <t>Yes *9</t>
-  </si>
-  <si>
-    <t>Clustered Indexes (data in heap)</t>
-  </si>
-  <si>
-    <t>Yes *17</t>
-  </si>
-  <si>
-    <t>Non-key columns on Indexes</t>
-  </si>
-  <si>
-    <t>Yes *8</t>
-  </si>
-  <si>
-    <t>Partial Indexes</t>
-  </si>
-  <si>
-    <t>SQL Optimization</t>
-  </si>
-  <si>
-    <t>Explain Plan</t>
-  </si>
-  <si>
-    <t>Explain Plan without execution</t>
-  </si>
-  <si>
-    <t>Explain Plan with parameters</t>
-  </si>
-  <si>
-    <t>Yes *1</t>
-  </si>
-  <si>
-    <t>Yes *5</t>
-  </si>
-  <si>
-    <t>Yes *6</t>
-  </si>
-  <si>
-    <t>*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
-  </si>
-  <si>
-    <t>*2 Informed by the database, but not used internally.</t>
-  </si>
-  <si>
-    <t>*3 The identifier can be typed in any case. It will match other cases.</t>
-  </si>
-  <si>
-    <t>*4 The identifier will be stored in the case it was typed.</t>
-  </si>
-  <si>
-    <t>*5 Yes, but the parameter types must be specified (not the values).</t>
-  </si>
-  <si>
-    <t>*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
-  </si>
-  <si>
-    <t>*7 Not enabled by default. The DBA needs to enable them after installation.</t>
-  </si>
-  <si>
-    <t>*8 On unique indexes only.</t>
-  </si>
-  <si>
-    <t>*9 Only on InnoDB tables.</t>
-  </si>
-  <si>
-    <t>*10 Can use user-defined functions since 10.2.1</t>
-  </si>
-  <si>
-    <t>*11 Only persistent virtual columns can be indexed.</t>
-  </si>
-  <si>
-    <t>*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
-  </si>
-  <si>
-    <t>*13 Always persisted.</t>
-  </si>
-  <si>
-    <t>*14 User-defined functions are not allowed.</t>
-  </si>
-  <si>
-    <t>*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
-  </si>
-  <si>
-    <t>*16 Must use deterministic UDFs.</t>
-  </si>
-  <si>
-    <t>*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
-  </si>
-  <si>
-    <t>*18 Are always persistent columns.</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="92">
+  <si>
+    <t xml:space="preserve">High End</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Middle Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighweight Tier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Organization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oracle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DB2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PostgreSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Server</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAP ASE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MariaDB</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MySQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Derby</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HyperSQL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Catalog Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">database</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CATALOG *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">catalog *2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Schema Term</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schema</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SCHEMA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identifier default case</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UPPER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lower</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insensitive *3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sensitive *4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Key Generation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sequences</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated always</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 12c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identities generated by default</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identity columns per table</t>
+  </si>
+  <si>
+    <t xml:space="preserve">single</t>
+  </si>
+  <si>
+    <t xml:space="preserve">multiple</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Extra Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hierarchical Queries</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 10.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From 8.0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Since 5.7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Full Text Search</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Expressions with UDF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indexes on Virtual Columns</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *11</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Optional indexes on FKs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Index Organized Tables (no heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clustered Indexes (data in heap)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Non-key columns on Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Partial Indexes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SQL Optimization</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan without execution</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Plan with parameters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes *6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*1 Yes, but requires to specify the type and one parameter value to get the explain plan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*2 Informed by the database, but not used internally.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*3 The identifier can be typed in any case. It will match other cases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*4 The identifier will be stored in the case it was typed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*5 Yes, but the parameter types must be specified (not the values).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*6 Yes, but MySQL and MariaDB sometimes fail to produce a plan for some parameters. If values are specified for those, the plan is retrieved successfully.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*7 Not enabled by default. The DBA needs to enable them after installation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*8 On unique indexes only.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*9 Only on InnoDB tables.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*10 Can use user-defined functions since 10.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*11 Only persistent virtual columns can be indexed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*12 The documentation says views cannot be created with hierarchical queries, but I could do it in H2 1.4.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*13 Always persisted.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*14 User-defined functions are not allowed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*15 PostgreSQL can emulate virtual columns as functions on a table (not persisted), However, they are not listed automatically when using * on a select.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*16 Must use deterministic UDFs.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*17 if the PK is a single column of type BIGINT, INT, SMALLINT, or TINYINT.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*18 Are always persistent columns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">*19 Only on materialized virtual columns.</t>
   </si>
 </sst>
 </file>
@@ -300,7 +303,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="GENERAL"/>
+    <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -573,22 +576,22 @@
   <dimension ref="A1:K47"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+      <selection pane="topLeft" activeCell="H32" activeCellId="0" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="31.1836734693878"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="11.0714285714286"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.2857142857143"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="30.780612244898"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.6071428571429"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="12" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -975,63 +978,63 @@
       <c r="E12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="G12" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="10" t="s">
+      <c r="H12" s="12" t="s">
         <v>42</v>
       </c>
-      <c r="H12" s="12" t="s">
+      <c r="I12" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="K12" s="10" t="s">
         <v>43</v>
-      </c>
-      <c r="I12" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="10" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="10" t="s">
         <v>45</v>
       </c>
-      <c r="B13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C13" s="10" t="s">
+      <c r="D13" s="15" t="s">
         <v>46</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E13" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F13" s="8" t="s">
-        <v>41</v>
-      </c>
-      <c r="G13" s="10" t="s">
+      <c r="H13" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I13" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="J13" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="K13" s="10" t="s">
         <v>49</v>
-      </c>
-      <c r="I13" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B14" s="8"/>
       <c r="C14" s="8"/>
@@ -1046,7 +1049,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B15" s="5" t="s">
         <v>4</v>
@@ -1081,7 +1084,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>30</v>
@@ -1116,11 +1119,11 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B17" s="10" t="s">
-        <v>55</v>
-      </c>
       <c r="C17" s="12" t="s">
         <v>31</v>
       </c>
@@ -1130,8 +1133,8 @@
       <c r="E17" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="8" t="s">
-        <v>41</v>
+      <c r="F17" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>31</v>
@@ -1151,22 +1154,22 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="F18" s="10" t="s">
         <v>56</v>
-      </c>
-      <c r="B18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="D18" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="F18" s="8" t="s">
-        <v>41</v>
       </c>
       <c r="G18" s="10" t="s">
         <v>57</v>
@@ -1200,8 +1203,8 @@
       <c r="E19" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F19" s="8" t="s">
-        <v>41</v>
+      <c r="F19" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G19" s="12" t="s">
         <v>31</v>
@@ -1235,8 +1238,8 @@
       <c r="E20" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="F20" s="8" t="s">
-        <v>41</v>
+      <c r="F20" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="G20" s="14" t="s">
         <v>60</v>
@@ -1270,8 +1273,8 @@
       <c r="E21" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F21" s="8" t="s">
-        <v>41</v>
+      <c r="F21" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G21" s="14" t="s">
         <v>60</v>
@@ -1305,8 +1308,8 @@
       <c r="E22" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F22" s="8" t="s">
-        <v>41</v>
+      <c r="F22" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="G22" s="12" t="s">
         <v>31</v>
@@ -1340,8 +1343,8 @@
       <c r="E23" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F23" s="8" t="s">
-        <v>41</v>
+      <c r="F23" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="G23" s="12" t="s">
         <v>31</v>
@@ -1410,8 +1413,8 @@
       <c r="E25" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F25" s="8" t="s">
-        <v>41</v>
+      <c r="F25" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G25" s="10" t="s">
         <v>30</v>
@@ -1445,8 +1448,8 @@
       <c r="E26" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>41</v>
+      <c r="F26" s="10" t="s">
+        <v>30</v>
       </c>
       <c r="G26" s="10" t="s">
         <v>30</v>
@@ -1480,8 +1483,8 @@
       <c r="E27" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="F27" s="8" t="s">
-        <v>41</v>
+      <c r="F27" s="12" t="s">
+        <v>31</v>
       </c>
       <c r="G27" s="14" t="s">
         <v>72</v>
@@ -1503,98 +1506,100 @@
       <c r="K28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>73</v>
+      </c>
       <c r="K29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="K30" s="0"/>
+        <v>74</v>
+      </c>
+      <c r="K30" s="16"/>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>74</v>
-      </c>
-      <c r="K31" s="16"/>
+        <v>75</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>